<commit_message>
acc changed DIRI and updated transect relative elevation information
</commit_message>
<xml_diff>
--- a/data/transect_info.xlsx
+++ b/data/transect_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\blopti_dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88917CEC-7AD3-44ED-BF39-DF5DB206CD57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277E5D4A-F4DA-4431-9F8D-DFACF8C7A395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="5400" windowWidth="28800" windowHeight="15435" xr2:uid="{B9BA70EB-BC33-4070-B6A6-DD3C8A1F4AB1}"/>
+    <workbookView xWindow="25620" yWindow="9465" windowWidth="12780" windowHeight="11535" xr2:uid="{B9BA70EB-BC33-4070-B6A6-DD3C8A1F4AB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>transect_length</t>
   </si>
@@ -129,6 +129,123 @@
   </si>
   <si>
     <t>transect_name</t>
+  </si>
+  <si>
+    <t>DAYUN 03</t>
+  </si>
+  <si>
+    <t>DAYUN 06</t>
+  </si>
+  <si>
+    <t>DAYUN 07</t>
+  </si>
+  <si>
+    <t>DAYUN 10</t>
+  </si>
+  <si>
+    <t>DAYUN 14</t>
+  </si>
+  <si>
+    <t>DAYUN 15</t>
+  </si>
+  <si>
+    <t>DAYUN 16</t>
+  </si>
+  <si>
+    <t>DAYUN 17</t>
+  </si>
+  <si>
+    <t>DAYUN 18</t>
+  </si>
+  <si>
+    <t>DAYUN 21</t>
+  </si>
+  <si>
+    <t>DAYUN 22</t>
+  </si>
+  <si>
+    <t>DAYUN 23</t>
+  </si>
+  <si>
+    <t>DAYUN 24</t>
+  </si>
+  <si>
+    <t>DAYUN 25</t>
+  </si>
+  <si>
+    <t>DAYUN 33</t>
+  </si>
+  <si>
+    <t>DAYUN 34</t>
+  </si>
+  <si>
+    <t>DAYUN 35</t>
+  </si>
+  <si>
+    <t>DAYUN 36</t>
+  </si>
+  <si>
+    <t>DAYUN 37</t>
+  </si>
+  <si>
+    <t>DAYUN 38</t>
+  </si>
+  <si>
+    <t>DOSAN 1</t>
+  </si>
+  <si>
+    <t>DOSAN 10</t>
+  </si>
+  <si>
+    <t>DOSAN 11</t>
+  </si>
+  <si>
+    <t>DOSAN 2</t>
+  </si>
+  <si>
+    <t>DOSAN 3</t>
+  </si>
+  <si>
+    <t>DOSAN 4</t>
+  </si>
+  <si>
+    <t>DOSAN 5</t>
+  </si>
+  <si>
+    <t>DOSAN 6</t>
+  </si>
+  <si>
+    <t>DOSAN 7</t>
+  </si>
+  <si>
+    <t>DOSAN 8</t>
+  </si>
+  <si>
+    <t>DOSAN 9</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>P009</t>
+  </si>
+  <si>
+    <t>P021</t>
+  </si>
+  <si>
+    <t>TNS1</t>
+  </si>
+  <si>
+    <t>TNT1</t>
+  </si>
+  <si>
+    <t>TNU1</t>
   </si>
 </sst>
 </file>
@@ -493,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFA8831-5967-4928-9040-44938CEAE61A}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,121 +652,317 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>-1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.11</v>
-      </c>
-      <c r="F2">
-        <v>120</v>
-      </c>
-      <c r="G2">
-        <v>-2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>-0.27</v>
-      </c>
-      <c r="F3">
-        <v>190</v>
-      </c>
-      <c r="G3">
-        <v>-8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>-1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>-0.22</v>
-      </c>
-      <c r="F4">
-        <v>127</v>
-      </c>
-      <c r="G4">
-        <v>-8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>-1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>-0.37</v>
-      </c>
-      <c r="F5">
-        <v>485</v>
-      </c>
-      <c r="G5">
-        <v>-8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>-1</v>
+      </c>
+      <c r="D33">
+        <v>0.11</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>120</v>
+      </c>
+      <c r="G33">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>-1</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0.27</v>
+      </c>
+      <c r="F38">
+        <v>190</v>
+      </c>
+      <c r="G38">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0.22</v>
+      </c>
+      <c r="F39">
+        <v>127</v>
+      </c>
+      <c r="G39">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>-1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.37</v>
+      </c>
+      <c r="F40">
+        <v>485</v>
+      </c>
+      <c r="G40">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
         <v>-1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>-0.24</v>
-      </c>
-      <c r="F6">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0.24</v>
+      </c>
+      <c r="F41">
         <v>210</v>
       </c>
-      <c r="G6">
+      <c r="G41">
         <v>-8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>